<commit_message>
Added an extra 100uF capacitor to +5_USB.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49CECE3-4F9C-431E-87BC-858CDCD1527C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C9F87-A03A-4A7F-A5BC-76193CB554B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp timestamp generator" sheetId="13" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="224">
   <si>
     <t>Value</t>
   </si>
@@ -86,9 +86,6 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>C0603</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>CRCW040210K0FKEDC</t>
   </si>
   <si>
-    <t>445-6899-2-ND</t>
-  </si>
-  <si>
     <t>CGA2B3X7R1H104K050BB</t>
   </si>
   <si>
@@ -209,12 +203,6 @@
     <t>CRCW040210R0FKEDHP</t>
   </si>
   <si>
-    <t>R54, R55</t>
-  </si>
-  <si>
-    <t>CRCW040210K0FKED</t>
-  </si>
-  <si>
     <t>R3, R7, R9, R14, R16, R18</t>
   </si>
   <si>
@@ -239,9 +227,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R21, R22, R23, R24, R25, R27, R28, R29, R30, R31</t>
-  </si>
-  <si>
     <t>CRCW04021K00FKED</t>
   </si>
   <si>
@@ -281,9 +266,6 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>A/3216-18W</t>
-  </si>
-  <si>
     <t>40R@100MHz</t>
   </si>
   <si>
@@ -581,9 +563,6 @@
     <t>311-330LRCT-ND</t>
   </si>
   <si>
-    <t>C10, C11, C23, C24</t>
-  </si>
-  <si>
     <t>350-1782-ND</t>
   </si>
   <si>
@@ -608,12 +587,6 @@
     <t>RC0603FR-07100KL</t>
   </si>
   <si>
-    <t>478-11183-1-ND</t>
-  </si>
-  <si>
-    <t>TAJA475K010TNJ</t>
-  </si>
-  <si>
     <t>563-1246-1-ND</t>
   </si>
   <si>
@@ -732,6 +705,42 @@
   </si>
   <si>
     <t>B2B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Battery lithium Polymer 2 Ah</t>
+  </si>
+  <si>
+    <t>MIKROE-1120</t>
+  </si>
+  <si>
+    <t>445-6899-1-ND</t>
+  </si>
+  <si>
+    <t>GRM155R61A334KE15D</t>
+  </si>
+  <si>
+    <t>490-3263-1-ND</t>
+  </si>
+  <si>
+    <t>R21, R22, R23, R24, R25, R27, R28, R29, R30, R31, R54, R55</t>
+  </si>
+  <si>
+    <t>C8, C10, C11, C23, C24</t>
+  </si>
+  <si>
+    <t>100u 25V</t>
+  </si>
+  <si>
+    <t>TT2D6</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>EEUFM1E101B</t>
+  </si>
+  <si>
+    <t>P19702CT-ND</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1244,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1266,6 +1275,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1633,13 +1645,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="17.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="35.140625" style="5" bestFit="1" customWidth="1"/>
@@ -1651,7 +1663,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1660,61 +1672,61 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="A2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1724,1151 +1736,1141 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
+      <c r="A5" s="4">
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>170</v>
+        <v>218</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>215</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>3</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="E39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>1</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>2</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>10</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>1</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E45" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>2</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>3</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="3" t="s">
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>1</v>
+      </c>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" t="s">
         <v>197</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>5</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>1</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>3</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>1</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>10</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>6</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>10</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>1</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>2</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>2</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>1</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>1</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>10</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>1</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>1</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
@@ -2877,14 +2879,14 @@
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F49" s="6"/>
-      <c r="G49"/>
-      <c r="H49"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
@@ -2893,14 +2895,14 @@
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E50" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F50" s="6"/>
-      <c r="G50"/>
-      <c r="H50"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
@@ -2909,14 +2911,20 @@
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51" t="s">
-        <v>208</v>
-      </c>
-      <c r="E51" t="s">
-        <v>209</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="G51"/>
-      <c r="H51"/>
+        <v>212</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H51" s="9">
+        <v>2786900</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
@@ -2925,64 +2933,64 @@
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F52" s="6"/>
-      <c r="G52"/>
-      <c r="H52"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
+      <c r="A53" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E54" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E55" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="7" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H55" s="9">
         <v>3712278</v>
@@ -2995,49 +3003,49 @@
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E56" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H56" s="10">
         <v>3402895</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
+      <c r="A57" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E58" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F58" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E59" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F59" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E60" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F60" s="1">
         <v>2</v>
@@ -3046,11 +3054,14 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A47:H47"/>
     <mergeCell ref="A57:H57"/>
     <mergeCell ref="A53:H53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B42" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added proper filtering to RESET line.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C9F87-A03A-4A7F-A5BC-76193CB554B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335202B6-45C9-4F45-BF5E-054C22FAB957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp timestamp generator" sheetId="13" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="228">
   <si>
     <t>Value</t>
   </si>
@@ -203,9 +203,6 @@
     <t>CRCW040210R0FKEDHP</t>
   </si>
   <si>
-    <t>R3, R7, R9, R14, R16, R18</t>
-  </si>
-  <si>
     <t>10n</t>
   </si>
   <si>
@@ -741,6 +738,21 @@
   </si>
   <si>
     <t>P19702CT-ND</t>
+  </si>
+  <si>
+    <t>R3, R7, R9, R14, R16, R18, R50</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>330pF</t>
+  </si>
+  <si>
+    <t>C0402C331J5GACTU</t>
+  </si>
+  <si>
+    <t>399-7787-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1643,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,16 +1716,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -1722,7 +1734,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1736,7 +1748,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>22</v>
@@ -1748,7 +1760,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1756,13 +1768,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>43</v>
@@ -1774,7 +1786,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1782,25 +1794,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1808,25 +1820,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1834,25 +1846,25 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1860,25 +1872,25 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1886,16 +1898,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>18</v>
@@ -1904,24 +1916,24 @@
         <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>104</v>
+        <v>225</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>105</v>
+        <v>224</v>
+      </c>
+      <c r="E11" t="s">
+        <v>226</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>19</v>
@@ -1930,24 +1942,24 @@
         <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>106</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>173</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>186</v>
+        <v>104</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>19</v>
@@ -1956,7 +1968,7 @@
         <v>15</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1964,16 +1976,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>132</v>
+        <v>185</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>19</v>
@@ -1982,44 +1994,44 @@
         <v>15</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>175</v>
@@ -2034,24 +2046,24 @@
         <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>19</v>
@@ -2060,7 +2072,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2068,16 +2080,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
@@ -2086,7 +2098,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2094,16 +2106,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>19</v>
@@ -2112,155 +2124,155 @@
         <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>2</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>3</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="F23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>5</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="F24" s="4" t="s">
         <v>19</v>
       </c>
@@ -2268,7 +2280,7 @@
         <v>15</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,25 +2288,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>191</v>
+        <v>135</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2302,25 +2314,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2328,16 +2340,16 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>19</v>
@@ -2346,7 +2358,7 @@
         <v>15</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2354,16 +2366,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>19</v>
@@ -2372,7 +2384,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2380,16 +2392,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>19</v>
@@ -2398,7 +2410,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2406,16 +2418,16 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="E30" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>19</v>
@@ -2424,7 +2436,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2432,16 +2444,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>19</v>
@@ -2450,24 +2462,24 @@
         <v>15</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>19</v>
@@ -2476,7 +2488,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2484,16 +2496,16 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>19</v>
@@ -2502,24 +2514,24 @@
         <v>15</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>208</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>209</v>
+        <v>73</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>19</v>
@@ -2528,51 +2540,51 @@
         <v>15</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="I34" s="5"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>12</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>217</v>
+        <v>42</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>19</v>
@@ -2581,24 +2593,24 @@
         <v>15</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>19</v>
@@ -2607,24 +2619,24 @@
         <v>15</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>56</v>
+        <v>223</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>19</v>
@@ -2633,24 +2645,24 @@
         <v>15</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>19</v>
@@ -2659,7 +2671,7 @@
         <v>15</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2667,16 +2679,16 @@
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>19</v>
@@ -2685,24 +2697,24 @@
         <v>15</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>171</v>
+        <v>48</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>19</v>
@@ -2711,33 +2723,33 @@
         <v>15</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>170</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2745,45 +2757,45 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>122</v>
+        <v>32</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>15</v>
@@ -2794,83 +2806,93 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="E46" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>1</v>
-      </c>
-      <c r="B46" s="3" t="s">
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="F47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
-        <v>1</v>
-      </c>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48" t="s">
-        <v>196</v>
-      </c>
-      <c r="E48" t="s">
-        <v>197</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="9"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
@@ -2879,10 +2901,10 @@
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="7"/>
@@ -2895,10 +2917,10 @@
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E50" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
@@ -2911,156 +2933,172 @@
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51" t="s">
-        <v>212</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="H51" s="9">
-        <v>2786900</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="E51" t="s">
+        <v>199</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" t="s">
+        <v>211</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H52" s="9">
+        <v>2786900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>4</v>
+      </c>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E52" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="9"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
-        <v>3</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54" t="s">
-        <v>193</v>
-      </c>
-      <c r="E54" t="s">
-        <v>194</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>195</v>
-      </c>
+      <c r="A54" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E55" t="s">
-        <v>204</v>
-      </c>
-      <c r="F55" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G55" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="H55" s="9">
-        <v>3712278</v>
+        <v>15</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56" t="s">
+        <v>202</v>
+      </c>
+      <c r="E56" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H56" s="9">
+        <v>3712278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>1</v>
+      </c>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57" t="s">
+        <v>204</v>
+      </c>
+      <c r="E57" t="s">
         <v>205</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G57" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H56" s="10">
+      <c r="H57" s="10">
         <v>3402895</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="1">
-        <v>44</v>
-      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E59" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F59" s="1">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E61" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="1">
-        <v>2</v>
+      <c r="F61" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A54:H54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B42" numberStoredAsText="1"/>
+    <ignoredError sqref="B43" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Corrected the discharge circuit.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335202B6-45C9-4F45-BF5E-054C22FAB957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AD373A-9F77-446A-BB45-53507E4C64F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp timestamp generator" sheetId="13" r:id="rId1"/>
@@ -719,9 +719,6 @@
     <t>490-3263-1-ND</t>
   </si>
   <si>
-    <t>R21, R22, R23, R24, R25, R27, R28, R29, R30, R31, R54, R55</t>
-  </si>
-  <si>
     <t>C8, C10, C11, C23, C24</t>
   </si>
   <si>
@@ -740,9 +737,6 @@
     <t>P19702CT-ND</t>
   </si>
   <si>
-    <t>R3, R7, R9, R14, R16, R18, R50</t>
-  </si>
-  <si>
     <t>C40</t>
   </si>
   <si>
@@ -753,6 +747,12 @@
   </si>
   <si>
     <t>399-7787-1-ND</t>
+  </si>
+  <si>
+    <t>R14, R21, R22, R23, R24, R25, R27, R28, R29, R30, R31, R54, R55</t>
+  </si>
+  <si>
+    <t>R3, R7, R9, R16, R18, R50</t>
   </si>
 </sst>
 </file>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1774,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>43</v>
@@ -1898,16 +1898,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>18</v>
@@ -1916,7 +1916,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1924,17 +1924,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" t="s">
         <v>224</v>
       </c>
-      <c r="E11" t="s">
-        <v>226</v>
-      </c>
       <c r="F11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2598,7 +2598,7 @@
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>50</v>
@@ -2607,7 +2607,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>51</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>10</v>
@@ -2633,7 +2633,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Decreased discharge current by ~60 mA to ~175 mA in average.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F3F3E-2561-4C12-BDC9-DBE0A3086700}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D46BA1-09B2-4440-B990-AF9F3D85DB81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="229">
   <si>
     <t>Value</t>
   </si>
@@ -689,12 +689,6 @@
     <t>Farnell</t>
   </si>
   <si>
-    <t>15R</t>
-  </si>
-  <si>
-    <t>CRM2512-FX-15R0ELF</t>
-  </si>
-  <si>
     <t>455-2247-ND</t>
   </si>
   <si>
@@ -753,6 +747,15 @@
   </si>
   <si>
     <t>Replacements: SI8621BB-B-IS</t>
+  </si>
+  <si>
+    <t>20R</t>
+  </si>
+  <si>
+    <t>CRM2512-FX-20R0ELF</t>
+  </si>
+  <si>
+    <t>118-CRM2512-FX-20R0ELFCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1661,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1673,7 @@
     <col min="5" max="5" width="23.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="1"/>
     <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1760,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1774,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>43</v>
@@ -1829,7 +1832,7 @@
         <v>58</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
@@ -1838,7 +1841,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1898,16 +1901,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>18</v>
@@ -1916,7 +1919,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1924,17 +1927,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" t="s">
         <v>221</v>
       </c>
-      <c r="E11" t="s">
-        <v>223</v>
-      </c>
       <c r="F11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2075,7 +2078,7 @@
         <v>144</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2551,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>52</v>
@@ -2560,7 +2563,7 @@
         <v>53</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>19</v>
@@ -2569,7 +2572,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="I35" s="5"/>
     </row>
@@ -2610,7 +2613,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>51</v>
@@ -2636,7 +2639,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>21</v>
@@ -2873,7 +2876,7 @@
         <v>86</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>19</v>
@@ -2882,7 +2885,7 @@
         <v>15</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2952,10 +2955,10 @@
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updated BOM and added front and rear panels.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D46BA1-09B2-4440-B990-AF9F3D85DB81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63284BEE-7096-40A8-AA03-A0AB1CB53C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp timestamp generator" sheetId="13" r:id="rId1"/>
@@ -164,12 +164,6 @@
     <t>PDI</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
     <t>100R</t>
   </si>
   <si>
@@ -572,12 +566,6 @@
     <t>IC5, IC11</t>
   </si>
   <si>
-    <t>311-0.0HRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0603FR-070RL</t>
-  </si>
-  <si>
     <t>311-100KHRCT-ND</t>
   </si>
   <si>
@@ -756,6 +744,18 @@
   </si>
   <si>
     <t>118-CRM2512-FX-20R0ELFCT-ND</t>
+  </si>
+  <si>
+    <t>Switch SPDT</t>
+  </si>
+  <si>
+    <t>7101MD9ABE</t>
+  </si>
+  <si>
+    <t>BATEN</t>
+  </si>
+  <si>
+    <t>CKN1045-ND</t>
   </si>
 </sst>
 </file>
@@ -1660,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,16 +1719,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -1737,7 +1737,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>22</v>
@@ -1763,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1771,16 +1771,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>19</v>
@@ -1789,7 +1789,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1797,17 +1797,17 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1823,16 +1823,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
@@ -1841,7 +1841,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1849,16 +1849,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>19</v>
@@ -1867,7 +1867,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1875,17 +1875,17 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1901,16 +1901,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>18</v>
@@ -1919,7 +1919,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1927,16 +1927,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>19</v>
@@ -1945,7 +1945,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1953,25 +1953,25 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1979,17 +1979,17 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="F13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>15</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2005,25 +2005,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="E14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2031,16 +2031,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>19</v>
@@ -2049,7 +2049,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2057,17 +2057,17 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="F16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2075,10 +2075,10 @@
         <v>15</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2086,25 +2086,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="E17" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2112,25 +2112,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2138,25 +2138,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="E19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2164,16 +2164,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>19</v>
@@ -2182,7 +2182,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2190,16 +2190,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>19</v>
@@ -2208,7 +2208,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2216,25 +2216,25 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="E22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2242,16 +2242,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>19</v>
@@ -2260,7 +2260,7 @@
         <v>15</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2268,17 +2268,17 @@
         <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F24" s="4" t="s">
         <v>19</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>15</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2294,25 +2294,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="E25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>29</v>
@@ -2329,7 +2329,7 @@
         <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>18</v>
@@ -2338,7 +2338,7 @@
         <v>15</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2346,25 +2346,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2372,25 +2372,25 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2398,25 +2398,25 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="E29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2424,25 +2424,25 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="E30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2450,25 +2450,25 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>9</v>
@@ -2485,7 +2485,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>19</v>
@@ -2494,7 +2494,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2502,25 +2502,25 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="E33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,17 +2528,17 @@
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="F34" s="4" t="s">
         <v>19</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>15</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2554,16 +2554,16 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>19</v>
@@ -2572,7 +2572,7 @@
         <v>15</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I35" s="5"/>
     </row>
@@ -2581,16 +2581,16 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>19</v>
@@ -2599,7 +2599,7 @@
         <v>15</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2607,16 +2607,16 @@
         <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>19</v>
@@ -2625,7 +2625,7 @@
         <v>15</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>21</v>
@@ -2659,16 +2659,16 @@
         <v>10</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>19</v>
@@ -2677,7 +2677,7 @@
         <v>15</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2685,17 +2685,17 @@
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="F40" s="4" t="s">
         <v>19</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>15</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2711,17 +2711,17 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="F41" s="4" t="s">
         <v>19</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>15</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2737,16 +2737,16 @@
         <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>19</v>
@@ -2755,7 +2755,7 @@
         <v>15</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2763,68 +2763,68 @@
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>19</v>
@@ -2833,7 +2833,7 @@
         <v>15</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2841,25 +2841,25 @@
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>158</v>
+        <v>226</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2867,16 +2867,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>19</v>
@@ -2885,7 +2885,7 @@
         <v>15</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2907,10 +2907,10 @@
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E49" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="7"/>
@@ -2923,10 +2923,10 @@
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
@@ -2939,10 +2939,10 @@
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E51" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="7"/>
@@ -2955,16 +2955,16 @@
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H52" s="9">
         <v>2786900</v>
@@ -2977,10 +2977,10 @@
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="7"/>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -3005,10 +3005,10 @@
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E55" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>16</v>
@@ -3017,7 +3017,7 @@
         <v>15</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3027,14 +3027,14 @@
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E56" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H56" s="9">
         <v>3712278</v>
@@ -3047,13 +3047,13 @@
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E57" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H57" s="10">
         <v>3402895</v>
@@ -3084,7 +3084,7 @@
         <v>12</v>
       </c>
       <c r="F60" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>11</v>
       </c>
       <c r="F61" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3104,9 +3104,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B43" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>